<commit_message>
Mudando a forma do projeto para PageObject e cadastro pela home com sucesso e falha, concluído
</commit_message>
<xml_diff>
--- a/target/MassaDados.xlsx
+++ b/target/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE065EEC-A95C-480C-8588-42486BD8D7CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBBA580-9E80-4ABD-BD1E-CEE7FB33473E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="1950" windowWidth="13410" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="131">
   <si>
     <t>email</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Bose Soundlink Bluetooth Speaker III</t>
   </si>
   <si>
-    <t>Dell Vostro</t>
-  </si>
-  <si>
     <t>HP USB 3 Button Optical Mouse</t>
   </si>
   <si>
@@ -410,6 +407,18 @@
   </si>
   <si>
     <t>(11)999537000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produto </t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>MICE</t>
   </si>
 </sst>
 </file>
@@ -812,467 +821,467 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1327,7 +1336,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -1396,7 +1405,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>19</v>
@@ -1405,19 +1414,19 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1435,7 +1444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB2D1F4-E107-4B1A-B01B-C8B4CC597D7B}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="C9:D9"/>
     </sheetView>
   </sheetViews>
@@ -1510,7 +1519,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>19</v>
@@ -1546,30 +1555,31 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -1585,24 +1595,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B601A69-DC0F-4ED2-9E8A-6A113BE67791}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>25</v>
-      </c>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1630,10 +1645,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -1669,7 +1684,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Busca pela lupa com sucesso e com falha, concluído
</commit_message>
<xml_diff>
--- a/target/MassaDados.xlsx
+++ b/target/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBBA580-9E80-4ABD-BD1E-CEE7FB33473E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B1FDA3-6E11-4CA2-AE92-7F54EE384C88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="7" r:id="rId1"/>
@@ -13,8 +13,8 @@
     <sheet name="CadastroFalha" sheetId="3" r:id="rId3"/>
     <sheet name="buscarHomeSucesso" sheetId="2" r:id="rId4"/>
     <sheet name="buscarHomeFalha" sheetId="4" r:id="rId5"/>
-    <sheet name="BuscaBarraSucesso" sheetId="5" r:id="rId6"/>
-    <sheet name="BuscaBarraFalha" sheetId="6" r:id="rId7"/>
+    <sheet name="BuscaLupaSucesso" sheetId="5" r:id="rId6"/>
+    <sheet name="BuscaLupaFalha" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="130">
   <si>
     <t>email</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Mouse Dell Supra</t>
-  </si>
-  <si>
-    <t>BRUN255</t>
   </si>
   <si>
     <t>Pais</t>
@@ -821,467 +818,467 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1333,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -1405,7 +1402,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>19</v>
@@ -1414,19 +1411,19 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1519,7 +1516,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>19</v>
@@ -1555,7 +1552,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1563,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>20</v>
@@ -1574,7 +1571,7 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>24</v>
@@ -1609,13 +1606,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="5"/>
     </row>
@@ -1630,7 +1627,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,12 +1644,7 @@
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1665,7 +1657,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refatoração para melhor funcionalidade do código
</commit_message>
<xml_diff>
--- a/target/MassaDados.xlsx
+++ b/target/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B1FDA3-6E11-4CA2-AE92-7F54EE384C88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2289D978-22AB-4C29-80BB-963598E6A23E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="136">
   <si>
     <t>email</t>
   </si>
@@ -415,7 +415,25 @@
     <t>Produto</t>
   </si>
   <si>
-    <t>MICE</t>
+    <t>Filtro</t>
+  </si>
+  <si>
+    <t>Escolha no filtro</t>
+  </si>
+  <si>
+    <t>Compatible with most notebook PCs, netbooks, tablets, mobile phones, and MP3 players with a 3.5 mm port available.</t>
+  </si>
+  <si>
+    <t>BY CONNECTOR</t>
+  </si>
+  <si>
+    <t>BlueTooth</t>
+  </si>
+  <si>
+    <t>HEADPHONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	BY COMPATIBILITY</t>
   </si>
 </sst>
 </file>
@@ -425,7 +443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,21 +493,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6F7FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE8E8E8"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -498,7 +537,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,6 +564,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1592,29 +1642,48 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B601A69-DC0F-4ED2-9E8A-6A113BE67791}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="C1" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="84.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
RGeralização do código para funcionar em vários funcionários
</commit_message>
<xml_diff>
--- a/target/MassaDados.xlsx
+++ b/target/MassaDados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2289D978-22AB-4C29-80BB-963598E6A23E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80D07B0-2B9F-4ABB-B445-CE2E33DBCF8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
     <t>HEADPHONES</t>
   </si>
   <si>
-    <t xml:space="preserve">	BY COMPATIBILITY</t>
+    <t>BY COMPATIBILITY</t>
   </si>
 </sst>
 </file>
@@ -1645,7 +1645,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>